<commit_message>
Added save functionality and updated documentation
</commit_message>
<xml_diff>
--- a/Excel_integration/testfakeecelresults.xlsx
+++ b/Excel_integration/testfakeecelresults.xlsx
@@ -456,60 +456,44 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>krawedz</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>inna_krawedz</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>krawedz</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>krawedz</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
poprawa buttonów, zakomentowanie niedokonczonych produkcji
</commit_message>
<xml_diff>
--- a/Excel_integration/testfakeecelresults.xlsx
+++ b/Excel_integration/testfakeecelresults.xlsx
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Pierwszy</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Drugi</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Trzeci</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Czwarty</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -459,13 +459,13 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>krawedz</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>inna_krawedz</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>krawedz</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -485,7 +485,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>krawedz</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>